<commit_message>
test case created api
</commit_message>
<xml_diff>
--- a/test_case_report/sprint_41.xlsx
+++ b/test_case_report/sprint_41.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\test_case_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499246AC-473B-4EFC-AF56-D508884AA353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1772E1B2-B984-475B-B48B-1FD39F03CE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -535,7 +535,7 @@
   <dimension ref="B2:C60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -798,16 +798,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B26:C26"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B50:C50"/>
     <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B26:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
api test case for use referral and referral code
</commit_message>
<xml_diff>
--- a/test_case_report/sprint_41.xlsx
+++ b/test_case_report/sprint_41.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\test_case_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8563EEE6-A945-4A4F-A138-296320D7E212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FD27F6-CFA3-4FCE-8436-C85CE13D597C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -644,19 +644,25 @@
       <c r="B21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2">
+        <v>3689</v>
+      </c>
     </row>
     <row r="22" spans="2:3" ht="18.75">
       <c r="B22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="4">
+        <v>1574</v>
+      </c>
     </row>
     <row r="23" spans="2:3" ht="18.75">
       <c r="B23" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="5">
+        <v>971</v>
+      </c>
     </row>
     <row r="26" spans="2:3" ht="18.75">
       <c r="B26" s="6" t="s">
@@ -804,16 +810,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B57:C57"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B57:C57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
learn api schema validation
</commit_message>
<xml_diff>
--- a/test_case_report/sprint_41.xlsx
+++ b/test_case_report/sprint_41.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\test_case_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE33A0B-9109-4CE6-87C3-05C780B1D793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24082060-8F0E-494A-B83D-55C5E8A3966E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -535,7 +535,7 @@
   <dimension ref="B2:C60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -735,7 +735,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="2">
-        <v>6730</v>
+        <v>6883</v>
       </c>
     </row>
     <row r="40" spans="2:3" ht="18.75">
@@ -828,16 +828,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B57:C57"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B57:C57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>